<commit_message>
Double spacing, saves FEDS version
</commit_message>
<xml_diff>
--- a/Paper/FEDSpaper/Figure descriptions.xlsx
+++ b/Paper/FEDSpaper/Figure descriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5604ff08deb8de49/Documents/Research/Denmark/IncomeUncertaintyGit/Paper/FEDSpaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="394" documentId="8_{F35E2840-29DF-4EB7-9F5E-397172B22ECF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{02A6ECCA-AF8E-4D0F-B200-D33F5F81A0BE}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{BE77B9D9-3289-41D8-827A-5B65C09AD704}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2F1FF051-FEFB-4C6B-A9AA-9B55A8201888}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0540149D-4974-4821-948C-194CD9D123CB}"/>
+    <workbookView xWindow="600" yWindow="858" windowWidth="14508" windowHeight="8790" xr2:uid="{0540149D-4974-4821-948C-194CD9D123CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure I" sheetId="1" r:id="rId1"/>
@@ -21,26 +21,23 @@
     <sheet name="Figure VI" sheetId="6" r:id="rId6"/>
     <sheet name="Figure VII" sheetId="7" r:id="rId7"/>
     <sheet name="Figure VIII" sheetId="8" r:id="rId8"/>
-    <sheet name="Figure IX" sheetId="9" r:id="rId9"/>
-    <sheet name="Figure X" sheetId="10" r:id="rId10"/>
-    <sheet name="Figure XI" sheetId="11" r:id="rId11"/>
-    <sheet name="Figure XII" sheetId="12" r:id="rId12"/>
-    <sheet name="Figure XIII" sheetId="13" r:id="rId13"/>
-    <sheet name="B.1" sheetId="14" r:id="rId14"/>
-    <sheet name="B.2" sheetId="15" r:id="rId15"/>
-    <sheet name="C.1" sheetId="16" r:id="rId16"/>
-    <sheet name="C.2" sheetId="17" r:id="rId17"/>
-    <sheet name="E.1" sheetId="18" r:id="rId18"/>
-    <sheet name="F.1" sheetId="19" r:id="rId19"/>
-    <sheet name="F.2" sheetId="20" r:id="rId20"/>
-    <sheet name="H.1" sheetId="21" r:id="rId21"/>
-    <sheet name="I.1" sheetId="22" r:id="rId22"/>
-    <sheet name="J.2" sheetId="23" r:id="rId23"/>
-    <sheet name="J.3" sheetId="24" r:id="rId24"/>
-    <sheet name="J.4" sheetId="25" r:id="rId25"/>
-    <sheet name="J.5" sheetId="26" r:id="rId26"/>
-    <sheet name="K.1" sheetId="27" r:id="rId27"/>
-    <sheet name="L.1" sheetId="28" r:id="rId28"/>
+    <sheet name="Figure IX" sheetId="12" r:id="rId9"/>
+    <sheet name="B.1" sheetId="14" r:id="rId10"/>
+    <sheet name="B.2" sheetId="15" r:id="rId11"/>
+    <sheet name="C.1" sheetId="16" r:id="rId12"/>
+    <sheet name="C.2" sheetId="17" r:id="rId13"/>
+    <sheet name="E.1" sheetId="18" r:id="rId14"/>
+    <sheet name="F.1" sheetId="13" r:id="rId15"/>
+    <sheet name="F.2" sheetId="20" r:id="rId16"/>
+    <sheet name="G.3" sheetId="29" r:id="rId17"/>
+    <sheet name="H.1" sheetId="21" r:id="rId18"/>
+    <sheet name="I.1" sheetId="22" r:id="rId19"/>
+    <sheet name="J.2" sheetId="23" r:id="rId20"/>
+    <sheet name="J.3" sheetId="24" r:id="rId21"/>
+    <sheet name="J.4" sheetId="25" r:id="rId22"/>
+    <sheet name="J.5" sheetId="26" r:id="rId23"/>
+    <sheet name="K.1" sheetId="27" r:id="rId24"/>
+    <sheet name="L.1" sheetId="28" r:id="rId25"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -58,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="85">
   <si>
     <t>Verbal description</t>
   </si>
@@ -177,24 +174,12 @@
     <t>Median Liquid Assets (USD)</t>
   </si>
   <si>
-    <t>The Lorenz curve shows cumulative liquid wealth share on the y-axis and percentile along the x-axis. The three target percentiles and cumulative shares are 20%, 0.0045; 40%, 0.0247; and 60%, 0.0793. The model Lorenz curve goes through these target points almost exactly. However, the model's Lorenz curve is below the Lorenz curve from the data at the 80th percentile.</t>
-  </si>
-  <si>
     <t>Top Left Panel</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Benchmark Model</t>
-  </si>
-  <si>
     <t>Top Right Panel</t>
   </si>
   <si>
-    <t>Preference Shock Model</t>
-  </si>
-  <si>
     <t>Verbal Description</t>
   </si>
   <si>
@@ -265,12 +250,6 @@
   </si>
   <si>
     <t>3) The estimates assuming exponential decay.  It shows the true permanent MPC is very closely approximated by the estimate.</t>
-  </si>
-  <si>
-    <t>Empirical Method</t>
-  </si>
-  <si>
-    <t>Model Partial Derivative (6m MPC)</t>
   </si>
   <si>
     <t>N</t>
@@ -989,541 +968,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC1CEE39-C0F8-4640-8C89-1BC7843D55F6}">
-  <dimension ref="A1:H18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="20.15625" customWidth="1"/>
-    <col min="3" max="3" width="15.47265625" customWidth="1"/>
-    <col min="5" max="5" width="21.47265625" customWidth="1"/>
-    <col min="7" max="7" width="19.9453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>0.83374060000000005</v>
-      </c>
-      <c r="C4">
-        <v>0.30972889749999999</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0.83374060000000005</v>
-      </c>
-      <c r="G4">
-        <v>0.59031146000000001</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>0.75251729999999994</v>
-      </c>
-      <c r="C5">
-        <v>0.2144128256</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>0.75251729999999994</v>
-      </c>
-      <c r="G5">
-        <v>0.479071527</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>0.55161280000000001</v>
-      </c>
-      <c r="C6">
-        <v>0.10350643380000001</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>0.55161280000000001</v>
-      </c>
-      <c r="G6">
-        <v>0.33781158700000002</v>
-      </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>0.4374905</v>
-      </c>
-      <c r="C7">
-        <v>3.7317751500000003E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>0.4374905</v>
-      </c>
-      <c r="G7">
-        <v>0.15965481400000001</v>
-      </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>0.23221310000000001</v>
-      </c>
-      <c r="C8">
-        <v>-1.5350720000000001E-4</v>
-      </c>
-      <c r="E8" s="2">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>0.23221310000000001</v>
-      </c>
-      <c r="G8">
-        <v>2.3238479999999999E-3</v>
-      </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>0.86624909999999999</v>
-      </c>
-      <c r="C14">
-        <v>1.0231730000000001</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>0.86624909999999999</v>
-      </c>
-      <c r="G14">
-        <v>1.0088957000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="1">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>0.75977309999999998</v>
-      </c>
-      <c r="C15">
-        <v>1.0302271000000001</v>
-      </c>
-      <c r="E15" s="1">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>0.75977309999999998</v>
-      </c>
-      <c r="G15">
-        <v>1.0198138999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="1">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>0.74159050000000004</v>
-      </c>
-      <c r="C16">
-        <v>1.0161058000000001</v>
-      </c>
-      <c r="E16" s="1">
-        <v>3</v>
-      </c>
-      <c r="F16">
-        <v>0.74159050000000004</v>
-      </c>
-      <c r="G16">
-        <v>1.0319111000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="1">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>0.67692509999999995</v>
-      </c>
-      <c r="C17">
-        <v>0.98671770000000003</v>
-      </c>
-      <c r="E17" s="1">
-        <v>4</v>
-      </c>
-      <c r="F17">
-        <v>0.67692509999999995</v>
-      </c>
-      <c r="G17">
-        <v>1.0203483</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2">
-        <v>5</v>
-      </c>
-      <c r="B18">
-        <v>0.57315530000000003</v>
-      </c>
-      <c r="C18">
-        <v>0.91932729999999996</v>
-      </c>
-      <c r="E18" s="2">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <v>0.57315530000000003</v>
-      </c>
-      <c r="G18">
-        <v>0.91401080000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38486800-050A-4D33-B7DB-C044EB738C96}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6E8FDE-331E-422C-9539-49E16067DAFB}">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="20.578125" customWidth="1"/>
-    <col min="2" max="2" width="13.9453125" customWidth="1"/>
-    <col min="3" max="3" width="15.41796875" customWidth="1"/>
-    <col min="4" max="4" width="14.26171875" customWidth="1"/>
-    <col min="5" max="5" width="13.62890625" customWidth="1"/>
-    <col min="6" max="6" width="14.9453125" customWidth="1"/>
-    <col min="7" max="7" width="15.7890625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>0.81660679999999997</v>
-      </c>
-      <c r="C3">
-        <v>0.81421920000000003</v>
-      </c>
-      <c r="D3">
-        <v>0.84631659999999997</v>
-      </c>
-      <c r="E3">
-        <v>0.82025380000000003</v>
-      </c>
-      <c r="F3">
-        <v>0.86970689999999995</v>
-      </c>
-      <c r="G3">
-        <v>0.82493039999999995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>0.70639439999999998</v>
-      </c>
-      <c r="C4">
-        <v>0.69001959999999996</v>
-      </c>
-      <c r="D4">
-        <v>0.74130980000000002</v>
-      </c>
-      <c r="E4">
-        <v>0.72857989999999995</v>
-      </c>
-      <c r="F4">
-        <v>0.7715225</v>
-      </c>
-      <c r="G4">
-        <v>0.75235160000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>0.6880676</v>
-      </c>
-      <c r="C5">
-        <v>0.4775933</v>
-      </c>
-      <c r="D5">
-        <v>0.72211599999999998</v>
-      </c>
-      <c r="E5">
-        <v>0.52536260000000001</v>
-      </c>
-      <c r="F5">
-        <v>0.75562110000000005</v>
-      </c>
-      <c r="G5">
-        <v>0.54611900000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>0.60268699999999997</v>
-      </c>
-      <c r="C6">
-        <v>0.38363039999999998</v>
-      </c>
-      <c r="D6">
-        <v>0.63975850000000001</v>
-      </c>
-      <c r="E6">
-        <v>0.42797489999999999</v>
-      </c>
-      <c r="F6">
-        <v>0.67621439999999999</v>
-      </c>
-      <c r="G6">
-        <v>0.4473298</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>0.50969690000000001</v>
-      </c>
-      <c r="C7">
-        <v>0.17409240000000001</v>
-      </c>
-      <c r="D7">
-        <v>0.52854089999999998</v>
-      </c>
-      <c r="E7">
-        <v>0.23413039999999999</v>
-      </c>
-      <c r="F7">
-        <v>0.5618088</v>
-      </c>
-      <c r="G7">
-        <v>0.24657989999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9D9984-E4CA-4884-960C-06806B6167A5}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96C7A12-238D-48B6-8A02-4FD2E420D445}">
   <dimension ref="A1:H44"/>
   <sheetViews>
@@ -1539,7 +983,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
@@ -1548,16 +992,16 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1571,16 +1015,16 @@
         <v>7.3462040000000003E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -1595,16 +1039,16 @@
         <v>6.7849629999999998E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2555,16 +1999,16 @@
         <v>2.270958E-3</v>
       </c>
       <c r="D43" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F43" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -2579,16 +2023,16 @@
         <v>1.8652880000000001E-3</v>
       </c>
       <c r="D44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H44" s="2"/>
     </row>
@@ -2597,7 +2041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F3BB9-62D0-4A0D-948E-3FB59E08D348}">
   <dimension ref="A1:E44"/>
   <sheetViews>
@@ -2607,7 +2051,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -3137,7 +2581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1E3A05-1BE1-4B09-9D3C-8F265F43BC63}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -3154,17 +2598,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -3172,7 +2616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5618D3C6-0E9B-4513-94F7-55F0568B0312}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -3189,17 +2633,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3207,7 +2651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF667043-7920-45FA-9D0C-A7F8E945B544}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -3298,12 +2742,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5809FB1-D00B-499F-9BF2-EEEC3268D317}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9D9984-E4CA-4884-960C-06806B6167A5}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3315,22 +2759,448 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F6CACD-7A3D-4BBB-98A3-02C29DDA038A}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="17.5234375" customWidth="1"/>
+    <col min="3" max="3" width="20.20703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4D988A-AFFE-41BF-BC99-BB1985198FF2}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7C2051-A0B7-426D-8AED-A95535180C33}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="17.47265625" customWidth="1"/>
+    <col min="4" max="4" width="19.62890625" customWidth="1"/>
+    <col min="5" max="5" width="26.15625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
         <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>4.5810549999999997E-3</v>
+      </c>
+      <c r="E2">
+        <v>2.7526059999999999E-3</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>6.3144270000000001E-3</v>
+      </c>
+      <c r="C3">
+        <v>7.5915150000000001E-3</v>
+      </c>
+      <c r="D3">
+        <v>4.315719E-3</v>
+      </c>
+      <c r="E3">
+        <v>5.1423770000000001E-3</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1.0338175999999999E-2</v>
+      </c>
+      <c r="C4">
+        <v>1.0601975E-2</v>
+      </c>
+      <c r="D4">
+        <v>7.489084E-3</v>
+      </c>
+      <c r="E4">
+        <v>7.5321470000000003E-3</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1.3679475999999999E-2</v>
+      </c>
+      <c r="C5">
+        <v>1.3612434E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.0064462999999999E-2</v>
+      </c>
+      <c r="E5">
+        <v>9.9219170000000006E-3</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1.6747621000000001E-2</v>
+      </c>
+      <c r="C6">
+        <v>1.6622893999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.2459507E-2</v>
+      </c>
+      <c r="E6">
+        <v>1.2311687999999999E-2</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1.9669181000000001E-2</v>
+      </c>
+      <c r="C7">
+        <v>1.9633352999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>1.4733671E-2</v>
+      </c>
+      <c r="E7">
+        <v>1.4701458000000001E-2</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2.2352354000000001E-2</v>
+      </c>
+      <c r="C8">
+        <v>2.2643812999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>1.6863230999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>1.7091228999999999E-2</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2.4870369E-2</v>
+      </c>
+      <c r="C9">
+        <v>2.5654272999999998E-2</v>
+      </c>
+      <c r="D9">
+        <v>1.8808113000000001E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.9480998999999999E-2</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2.740304E-2</v>
+      </c>
+      <c r="C10">
+        <v>2.8664731999999998E-2</v>
+      </c>
+      <c r="D10">
+        <v>2.0678153000000001E-2</v>
+      </c>
+      <c r="E10">
+        <v>2.1870769000000002E-2</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>3.0161078000000001E-2</v>
+      </c>
+      <c r="C11">
+        <v>3.1675191999999998E-2</v>
+      </c>
+      <c r="D11">
+        <v>2.266396E-2</v>
+      </c>
+      <c r="E11">
+        <v>2.4260540000000001E-2</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>3.3129248E-2</v>
+      </c>
+      <c r="C12">
+        <v>3.4685650999999998E-2</v>
+      </c>
+      <c r="D12">
+        <v>2.4798448000000001E-2</v>
+      </c>
+      <c r="E12">
+        <v>2.665031E-2</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3840BB50-5CBB-498E-88B0-E1FB3F20160A}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>2004</v>
+      </c>
+      <c r="B2">
+        <v>8.7332499999999993E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2005</v>
+      </c>
+      <c r="B3">
+        <v>8.8220900000000005E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>2006</v>
+      </c>
+      <c r="B4">
+        <v>8.7484999999999993E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2007</v>
+      </c>
+      <c r="B5">
+        <v>9.3144500000000005E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>2008</v>
+      </c>
+      <c r="B6">
+        <v>9.2650800000000005E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>2009</v>
+      </c>
+      <c r="B7">
+        <v>9.4964199999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>2010</v>
+      </c>
+      <c r="B8">
+        <v>9.6026700000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>2011</v>
+      </c>
+      <c r="B9">
+        <v>9.1331499999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>2012</v>
+      </c>
+      <c r="B10">
+        <v>8.69201E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>2013</v>
+      </c>
+      <c r="B11">
+        <v>8.6165099999999994E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>8.5333099999999995E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>2015</v>
+      </c>
+      <c r="B13">
+        <v>8.6575200000000005E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3364,451 +3234,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F6CACD-7A3D-4BBB-98A3-02C29DDA038A}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="2" max="2" width="17.5234375" customWidth="1"/>
-    <col min="3" max="3" width="20.20703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0.59031146000000001</v>
-      </c>
-      <c r="C2">
-        <v>0.59641840999999995</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0.479071527</v>
-      </c>
-      <c r="C3">
-        <v>0.52479487000000002</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0.33781158700000002</v>
-      </c>
-      <c r="C4">
-        <v>0.44926384000000003</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0.15965481400000001</v>
-      </c>
-      <c r="C5">
-        <v>0.32996798999999999</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2.3238479999999999E-3</v>
-      </c>
-      <c r="C6">
-        <v>4.8001670000000003E-2</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7C2051-A0B7-426D-8AED-A95535180C33}">
-  <dimension ref="A1:G12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="2" max="2" width="17.47265625" customWidth="1"/>
-    <col min="4" max="4" width="19.62890625" customWidth="1"/>
-    <col min="5" max="5" width="26.15625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>4.5810549999999997E-3</v>
-      </c>
-      <c r="E2">
-        <v>2.7526059999999999E-3</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>6.3144270000000001E-3</v>
-      </c>
-      <c r="C3">
-        <v>7.5915150000000001E-3</v>
-      </c>
-      <c r="D3">
-        <v>4.315719E-3</v>
-      </c>
-      <c r="E3">
-        <v>5.1423770000000001E-3</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1.0338175999999999E-2</v>
-      </c>
-      <c r="C4">
-        <v>1.0601975E-2</v>
-      </c>
-      <c r="D4">
-        <v>7.489084E-3</v>
-      </c>
-      <c r="E4">
-        <v>7.5321470000000003E-3</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1.3679475999999999E-2</v>
-      </c>
-      <c r="C5">
-        <v>1.3612434E-2</v>
-      </c>
-      <c r="D5">
-        <v>1.0064462999999999E-2</v>
-      </c>
-      <c r="E5">
-        <v>9.9219170000000006E-3</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>1.6747621000000001E-2</v>
-      </c>
-      <c r="C6">
-        <v>1.6622893999999999E-2</v>
-      </c>
-      <c r="D6">
-        <v>1.2459507E-2</v>
-      </c>
-      <c r="E6">
-        <v>1.2311687999999999E-2</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>1.9669181000000001E-2</v>
-      </c>
-      <c r="C7">
-        <v>1.9633352999999999E-2</v>
-      </c>
-      <c r="D7">
-        <v>1.4733671E-2</v>
-      </c>
-      <c r="E7">
-        <v>1.4701458000000001E-2</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>2.2352354000000001E-2</v>
-      </c>
-      <c r="C8">
-        <v>2.2643812999999999E-2</v>
-      </c>
-      <c r="D8">
-        <v>1.6863230999999999E-2</v>
-      </c>
-      <c r="E8">
-        <v>1.7091228999999999E-2</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>2.4870369E-2</v>
-      </c>
-      <c r="C9">
-        <v>2.5654272999999998E-2</v>
-      </c>
-      <c r="D9">
-        <v>1.8808113000000001E-2</v>
-      </c>
-      <c r="E9">
-        <v>1.9480998999999999E-2</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>2.740304E-2</v>
-      </c>
-      <c r="C10">
-        <v>2.8664731999999998E-2</v>
-      </c>
-      <c r="D10">
-        <v>2.0678153000000001E-2</v>
-      </c>
-      <c r="E10">
-        <v>2.1870769000000002E-2</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>3.0161078000000001E-2</v>
-      </c>
-      <c r="C11">
-        <v>3.1675191999999998E-2</v>
-      </c>
-      <c r="D11">
-        <v>2.266396E-2</v>
-      </c>
-      <c r="E11">
-        <v>2.4260540000000001E-2</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>3.3129248E-2</v>
-      </c>
-      <c r="C12">
-        <v>3.4685650999999998E-2</v>
-      </c>
-      <c r="D12">
-        <v>2.4798448000000001E-2</v>
-      </c>
-      <c r="E12">
-        <v>2.665031E-2</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3840BB50-5CBB-498E-88B0-E1FB3F20160A}">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>2004</v>
-      </c>
-      <c r="B2">
-        <v>8.7332499999999993E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>2005</v>
-      </c>
-      <c r="B3">
-        <v>8.8220900000000005E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>2006</v>
-      </c>
-      <c r="B4">
-        <v>8.7484999999999993E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>2007</v>
-      </c>
-      <c r="B5">
-        <v>9.3144500000000005E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>2008</v>
-      </c>
-      <c r="B6">
-        <v>9.2650800000000005E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
-        <v>2009</v>
-      </c>
-      <c r="B7">
-        <v>9.4964199999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
-        <v>2010</v>
-      </c>
-      <c r="B8">
-        <v>9.6026700000000006E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
-        <v>2011</v>
-      </c>
-      <c r="B9">
-        <v>9.1331499999999996E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <v>2012</v>
-      </c>
-      <c r="B10">
-        <v>8.69201E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
-        <v>2013</v>
-      </c>
-      <c r="B11">
-        <v>8.6165099999999994E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
-        <v>2014</v>
-      </c>
-      <c r="B12">
-        <v>8.5333099999999995E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
-        <v>2015</v>
-      </c>
-      <c r="B13">
-        <v>8.6575200000000005E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACA0AF8-2BC2-498C-B2D3-3F83EA66C5E9}">
   <dimension ref="A1:K7"/>
   <sheetViews>
@@ -3820,10 +3245,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3831,31 +3256,31 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -4008,7 +3433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9349244E-5545-4F90-AB0A-29C3D5C20F55}">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -4020,10 +3445,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -4031,19 +3456,19 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" t="s">
-        <v>85</v>
-      </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" t="s">
         <v>79</v>
-      </c>
-      <c r="I2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -4206,7 +3631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D889091-989A-4F87-8E59-B500B3CDD4D9}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -4218,13 +3643,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -4342,7 +3767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87B9879-9D66-4920-A15C-0E2729F39783}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -4357,10 +3782,10 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -4423,7 +3848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DD5CC7-0661-4F9C-AE3B-3BA48A6A132E}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -4443,10 +3868,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
         <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4811,7 +4236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD92321-F4BF-4A73-805C-1EBFD4D7B179}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -4826,16 +4251,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5614,23 +5039,171 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7CD4D7-4324-479B-93AA-F9F70F7E5297}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6E8FDE-331E-422C-9539-49E16067DAFB}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="20.578125" customWidth="1"/>
+    <col min="2" max="2" width="13.9453125" customWidth="1"/>
+    <col min="3" max="3" width="15.41796875" customWidth="1"/>
+    <col min="4" max="4" width="14.26171875" customWidth="1"/>
+    <col min="5" max="5" width="13.62890625" customWidth="1"/>
+    <col min="6" max="6" width="14.9453125" customWidth="1"/>
+    <col min="7" max="7" width="15.7890625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>0.81660679999999997</v>
+      </c>
+      <c r="C3">
+        <v>0.81421920000000003</v>
+      </c>
+      <c r="D3">
+        <v>0.84631659999999997</v>
+      </c>
+      <c r="E3">
+        <v>0.82025380000000003</v>
+      </c>
+      <c r="F3">
+        <v>0.86970689999999995</v>
+      </c>
+      <c r="G3">
+        <v>0.82493039999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0.70639439999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.69001959999999996</v>
+      </c>
+      <c r="D4">
+        <v>0.74130980000000002</v>
+      </c>
+      <c r="E4">
+        <v>0.72857989999999995</v>
+      </c>
+      <c r="F4">
+        <v>0.7715225</v>
+      </c>
+      <c r="G4">
+        <v>0.75235160000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0.6880676</v>
+      </c>
+      <c r="C5">
+        <v>0.4775933</v>
+      </c>
+      <c r="D5">
+        <v>0.72211599999999998</v>
+      </c>
+      <c r="E5">
+        <v>0.52536260000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.75562110000000005</v>
+      </c>
+      <c r="G5">
+        <v>0.54611900000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>0.60268699999999997</v>
+      </c>
+      <c r="C6">
+        <v>0.38363039999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.63975850000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.42797489999999999</v>
+      </c>
+      <c r="F6">
+        <v>0.67621439999999999</v>
+      </c>
+      <c r="G6">
+        <v>0.4473298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>0.50969690000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.17409240000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.52854089999999998</v>
+      </c>
+      <c r="E7">
+        <v>0.23413039999999999</v>
+      </c>
+      <c r="F7">
+        <v>0.5618088</v>
+      </c>
+      <c r="G7">
+        <v>0.24657989999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>